<commit_message>
added comments and updated some of the code so that it worked "better"
</commit_message>
<xml_diff>
--- a/CreateExcelWorksheet/CreateExcelWorksheet/SalesByWeekly.xlsx
+++ b/CreateExcelWorksheet/CreateExcelWorksheet/SalesByWeekly.xlsx
@@ -2,6 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileSharing readOnlyRecommended="1"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="18195" windowHeight="7740" activeTab="1"/>
@@ -1774,511 +1775,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
-      <c:rAngAx val="1"/>
-    </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-    </c:backWall>
-    <c:plotArea>
-      <c:layout/>
-      <c:bar3DChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:invertIfNegative val="0"/>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="00B0F0"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="8"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="9"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="10"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="00B050"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="1.5996800639872025E-3"/>
-                  <c:y val="-2.2695035460992909E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0"/>
-                  <c:y val="-1.7021276595744681E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="1.5996800639871732E-3"/>
-                  <c:y val="-1.7021276595744681E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="3.9992001599680064E-3"/>
-                  <c:y val="-2.4586288416075651E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0"/>
-                  <c:y val="-1.1347517730496455E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="5.8654258100536017E-17"/>
-                  <c:y val="-1.7021276595744681E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="6"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="5.8654258100536017E-17"/>
-                  <c:y val="-1.3238770685579196E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="7"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="7.9984003199360125E-4"/>
-                  <c:y val="-1.8912529550827423E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="8"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="7.9984003199360125E-4"/>
-                  <c:y val="-1.7021276595744681E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="9"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0"/>
-                  <c:y val="-1.3238770685579196E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="10"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0"/>
-                  <c:y val="-1.1347517730496453E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:spPr/>
-              <c:txPr>
-                <a:bodyPr/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1400" b="1">
-                      <a:solidFill>
-                        <a:srgbClr val="00B050"/>
-                      </a:solidFill>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="11"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0"/>
-                  <c:y val="-1.1347517730496455E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:spPr/>
-              <c:txPr>
-                <a:bodyPr/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1400" b="1">
-                      <a:solidFill>
-                        <a:srgbClr val="FF0000"/>
-                      </a:solidFill>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-            </c:dLbl>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1400" b="1">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1"/>
-                    </a:solidFill>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Shipment-ByCell per week'!$C$1:$N$1</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>CHUCKER</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>MILL</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>SHORTRN</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>SOD/GEN</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>SWISS</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>TWIN</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>VALVE</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>WEEKLY ACTUAL TOTAL</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>SCHEDULED WEEKLY SALES</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>WEEKLY FORECAST</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>MONTH TO DATE SALES</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>SALES GOAL MONTHLY</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Shipment-ByCell per week'!$C$2:$N$2</c:f>
-              <c:numCache>
-                <c:formatCode>"$"#,##0.00</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>25542.95</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>48656.34</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5328.13</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20154.48</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6895</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>28254</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>27716.070000000003</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>162546.97</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>290461.41000000003</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>250000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>443684.25</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1000000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:shape val="box"/>
-        <c:axId val="123620352"/>
-        <c:axId val="123630336"/>
-        <c:axId val="0"/>
-      </c:bar3DChart>
-      <c:catAx>
-        <c:axId val="123620352"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123630336"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="123630336"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="&quot;$&quot;#,##0.00" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123620352"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:ln>
-      <a:gradFill>
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="accent1">
-              <a:tint val="66000"/>
-              <a:satMod val="160000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="50000">
-            <a:schemeClr val="accent1">
-              <a:tint val="44500"/>
-              <a:satMod val="160000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="accent1">
-              <a:tint val="23500"/>
-              <a:satMod val="160000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="0"/>
-      </a:gradFill>
-    </a:ln>
-    <a:effectLst>
-      <a:glow rad="127000">
-        <a:schemeClr val="bg2">
-          <a:lumMod val="90000"/>
-        </a:schemeClr>
-      </a:glow>
-    </a:effectLst>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-  <c:userShapes r:id="rId1"/>
-</c:chartSpace>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3233,201 +2729,6 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.11292</cdr:x>
-      <cdr:y>0.03156</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.52398</cdr:x>
-      <cdr:y>0.17178</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="2" name="Rectangle 1"/>
-        <cdr:cNvSpPr/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1684403" y="211004"/>
-          <a:ext cx="6131432" cy="937588"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="5400" b="1" cap="none" spc="300">
-              <a:ln w="11430" cmpd="sng">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:tint val="10000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-                <a:miter lim="800000"/>
-              </a:ln>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="10000">
-                    <a:schemeClr val="accent1">
-                      <a:tint val="83000"/>
-                      <a:shade val="100000"/>
-                      <a:satMod val="200000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="75000">
-                    <a:schemeClr val="accent1">
-                      <a:tint val="100000"/>
-                      <a:shade val="50000"/>
-                      <a:satMod val="150000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000"/>
-              </a:gradFill>
-              <a:effectLst>
-                <a:glow rad="45500">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="220000"/>
-                    <a:alpha val="35000"/>
-                  </a:schemeClr>
-                </a:glow>
-              </a:effectLst>
-            </a:rPr>
-            <a:t>Weekly</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="5400" b="1" cap="none" spc="300" baseline="0">
-              <a:ln w="11430" cmpd="sng">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:tint val="10000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-                <a:miter lim="800000"/>
-              </a:ln>
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="10000">
-                    <a:schemeClr val="accent1">
-                      <a:tint val="83000"/>
-                      <a:shade val="100000"/>
-                      <a:satMod val="200000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="75000">
-                    <a:schemeClr val="accent1">
-                      <a:tint val="100000"/>
-                      <a:shade val="50000"/>
-                      <a:satMod val="150000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000"/>
-              </a:gradFill>
-              <a:effectLst>
-                <a:glow rad="45500">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="220000"/>
-                    <a:alpha val="35000"/>
-                  </a:schemeClr>
-                </a:glow>
-              </a:effectLst>
-            </a:rPr>
-            <a:t> Sales Data</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="5400" b="1" cap="none" spc="300">
-            <a:ln w="11430" cmpd="sng">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:tint val="10000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:miter lim="800000"/>
-            </a:ln>
-            <a:gradFill>
-              <a:gsLst>
-                <a:gs pos="10000">
-                  <a:schemeClr val="accent1">
-                    <a:tint val="83000"/>
-                    <a:shade val="100000"/>
-                    <a:satMod val="200000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="75000">
-                  <a:schemeClr val="accent1">
-                    <a:tint val="100000"/>
-                    <a:shade val="50000"/>
-                    <a:satMod val="150000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000"/>
-            </a:gradFill>
-            <a:effectLst>
-              <a:glow rad="45500">
-                <a:schemeClr val="accent1">
-                  <a:satMod val="220000"/>
-                  <a:alpha val="35000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
-          </a:endParaRPr>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-</c:userShapes>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
@@ -6052,21 +5353,21 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="15">
+    <mergeCell ref="U11:U12"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="U15:U16"/>
+    <mergeCell ref="U17:U18"/>
+    <mergeCell ref="U19:U20"/>
+    <mergeCell ref="U30:U31"/>
+    <mergeCell ref="U32:U33"/>
+    <mergeCell ref="U34:U35"/>
+    <mergeCell ref="U36:U37"/>
+    <mergeCell ref="U28:U29"/>
     <mergeCell ref="U45:U46"/>
     <mergeCell ref="U47:U48"/>
     <mergeCell ref="U49:U50"/>
     <mergeCell ref="U51:U52"/>
     <mergeCell ref="U53:U54"/>
-    <mergeCell ref="U30:U31"/>
-    <mergeCell ref="U32:U33"/>
-    <mergeCell ref="U34:U35"/>
-    <mergeCell ref="U36:U37"/>
-    <mergeCell ref="U28:U29"/>
-    <mergeCell ref="U11:U12"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="U15:U16"/>
-    <mergeCell ref="U17:U18"/>
-    <mergeCell ref="U19:U20"/>
   </mergeCells>
   <conditionalFormatting sqref="U11:U20">
     <cfRule type="cellIs" dxfId="36" priority="5" operator="greaterThan">
@@ -6443,7 +5744,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
@@ -6716,7 +6017,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>